<commit_message>
project 2 grinding and adding a test scratchwork folder
</commit_message>
<xml_diff>
--- a/projects/cs2200-project-2-early/microcode.xlsx
+++ b/projects/cs2200-project-2-early/microcode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="129">
   <si>
     <t xml:space="preserve">Index</t>
   </si>
@@ -395,7 +395,7 @@
     <t xml:space="preserve">0111</t>
   </si>
   <si>
-    <t xml:space="preserve">what?</t>
+    <t xml:space="preserve">6</t>
   </si>
   <si>
     <t xml:space="preserve">blt</t>
@@ -689,7 +689,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -729,7 +729,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -753,7 +753,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,13 +914,13 @@
   </sheetPr>
   <dimension ref="A1:AS1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AC40" activeCellId="0" sqref="AC40"/>
+      <selection pane="bottomLeft" activeCell="K67" activeCellId="0" sqref="K67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.79"/>
@@ -7577,8 +7577,7 @@
       <c r="I68" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J68" s="24" t="str">
-        <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C68)</f>
+      <c r="J68" s="24" t="n">
         <v>1</v>
       </c>
       <c r="M68" s="19" t="s">
@@ -7604,18 +7603,20 @@
       <c r="B69" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C69" s="22"/>
+      <c r="C69" s="22" t="s">
+        <v>111</v>
+      </c>
       <c r="D69" s="22"/>
       <c r="E69" s="22"/>
       <c r="F69" s="22"/>
       <c r="G69" s="22"/>
       <c r="H69" s="22"/>
       <c r="I69" s="23" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="J69" s="24" t="str">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getDec2Hex(C69)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M69" s="19" t="s">
         <v>112</v>

</xml_diff>